<commit_message>
Project clean up for the final upload
</commit_message>
<xml_diff>
--- a/Dataset_Lean_h0/Dataset_h0.xlsx
+++ b/Dataset_Lean_h0/Dataset_h0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filippo\Documents\Proj inz\Dataset_Lean_h0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37429DB-4F6A-484C-A7D7-620C096DBA49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5489CF1A-5CB5-4351-8802-EBADF18B3F5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-2190" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Img</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Suma:</t>
+  </si>
+  <si>
+    <t>PET Img/ Img</t>
   </si>
 </sst>
 </file>
@@ -174,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -228,13 +231,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -242,6 +239,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -2392,7 +2399,7 @@
   <dimension ref="A2:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2404,7 +2411,7 @@
     <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="10" t="s">
         <v>8</v>
@@ -2424,8 +2431,11 @@
       <c r="G2" s="10" t="s">
         <v>10</v>
       </c>
+      <c r="H2" s="23" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
@@ -2439,18 +2449,25 @@
         <v>3.8</v>
       </c>
       <c r="E3" s="3">
-        <f>(C3-B3*(1-(G3/100))*4)</f>
+        <f t="shared" ref="E3:E8" si="0">(C3-B3*(1-(G3/100))*4)</f>
         <v>207.22</v>
       </c>
       <c r="F3" s="3">
-        <f>C3-(C3-B3*(1-(G3/100))*4)</f>
+        <f t="shared" ref="F3:F8" si="1">C3-(C3-B3*(1-(G3/100))*4)</f>
         <v>219.78</v>
       </c>
       <c r="G3" s="2">
         <v>50.5</v>
       </c>
+      <c r="H3" s="24">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <f>C3*H3</f>
+        <v>427</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -2464,18 +2481,25 @@
         <v>3.3</v>
       </c>
       <c r="E4" s="13">
-        <f>(C4-B4*(1-(G4/100))*4)</f>
+        <f t="shared" si="0"/>
         <v>28.951999999999998</v>
       </c>
       <c r="F4" s="13">
-        <f>C4-(C4-B4*(1-(G4/100))*4)</f>
+        <f t="shared" si="1"/>
         <v>60.048000000000002</v>
       </c>
       <c r="G4" s="12">
         <v>44.4</v>
       </c>
+      <c r="H4" s="24">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I8" si="2">C4*H4</f>
+        <v>356</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
@@ -2489,18 +2513,25 @@
         <v>4</v>
       </c>
       <c r="E5" s="13">
-        <f>(C5-B5*(1-(G5/100))*4)</f>
+        <f t="shared" si="0"/>
         <v>76</v>
       </c>
       <c r="F5" s="13">
-        <f>C5-(C5-B5*(1-(G5/100))*4)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G5" s="12">
         <v>100</v>
       </c>
+      <c r="H5" s="24">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <f>C5*H5</f>
+        <v>304</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -2514,18 +2545,25 @@
         <v>3.9</v>
       </c>
       <c r="E6" s="13">
-        <f>(C6-B6*(1-(G6/100))*4)</f>
+        <f t="shared" si="0"/>
         <v>310.096</v>
       </c>
       <c r="F6" s="13">
-        <f>C6-(C6-B6*(1-(G6/100))*4)</f>
+        <f t="shared" si="1"/>
         <v>59.903999999999996</v>
       </c>
       <c r="G6" s="12">
         <v>84.4</v>
       </c>
+      <c r="H6" s="24">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>370</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
@@ -2539,18 +2577,25 @@
         <v>3.9</v>
       </c>
       <c r="E7" s="13">
-        <f>(C7-B7*(1-(G7/100))*4)</f>
+        <f t="shared" si="0"/>
         <v>61.952000000000005</v>
       </c>
       <c r="F7" s="13">
-        <f>C7-(C7-B7*(1-(G7/100))*4)</f>
+        <f t="shared" si="1"/>
         <v>48.047999999999995</v>
       </c>
       <c r="G7" s="12">
         <v>57.1</v>
       </c>
+      <c r="H7" s="24">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>330</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>6</v>
       </c>
@@ -2564,18 +2609,25 @@
         <v>3.8</v>
       </c>
       <c r="E8" s="13">
-        <f>(C8-B8*(1-(G8/100))*4)</f>
+        <f t="shared" si="0"/>
         <v>94</v>
       </c>
       <c r="F8" s="13">
-        <f>C8-(C8-B8*(1-(G8/100))*4)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G8" s="1">
         <v>100</v>
       </c>
+      <c r="H8" s="24">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>376</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -2592,11 +2644,11 @@
         <v>3.7833333333333332</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" ref="E9:F9" si="0">SUM(E3:E8)</f>
+        <f t="shared" ref="E9:F9" si="3">SUM(E3:E8)</f>
         <v>778.22</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>387.78</v>
       </c>
       <c r="G9" s="14">
@@ -2605,11 +2657,11 @@
       </c>
     </row>
     <row r="18" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I18" s="18"/>
-      <c r="J18" s="19" t="s">
+      <c r="I18" s="22"/>
+      <c r="J18" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="19" t="s">
+      <c r="K18" s="18" t="s">
         <v>14</v>
       </c>
       <c r="L18" s="17" t="s">
@@ -2623,17 +2675,17 @@
       </c>
     </row>
     <row r="19" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I19" s="18"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
       <c r="L19" s="17"/>
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
     </row>
     <row r="20" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I20" s="18"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
       <c r="L20" s="17" t="s">
         <v>15</v>
       </c>
@@ -2645,238 +2697,215 @@
       </c>
     </row>
     <row r="21" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I21" s="18"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
       <c r="L21" s="16"/>
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
     </row>
     <row r="22" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="20">
+      <c r="J22" s="21">
         <v>111</v>
       </c>
-      <c r="K22" s="20">
+      <c r="K22" s="21">
         <v>427</v>
       </c>
-      <c r="L22" s="20">
+      <c r="L22" s="21">
         <v>4</v>
       </c>
-      <c r="M22" s="20">
+      <c r="M22" s="21">
         <v>207</v>
       </c>
-      <c r="N22" s="20">
+      <c r="N22" s="21">
         <v>220</v>
       </c>
     </row>
     <row r="23" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I23" s="19"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="21"/>
     </row>
     <row r="24" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I24" s="19" t="s">
+      <c r="I24" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="J24" s="20">
+      <c r="J24" s="21">
         <v>27</v>
       </c>
-      <c r="K24" s="20">
+      <c r="K24" s="21">
         <v>89</v>
       </c>
-      <c r="L24" s="20">
+      <c r="L24" s="21">
         <v>3</v>
       </c>
-      <c r="M24" s="20">
+      <c r="M24" s="21">
         <v>29</v>
       </c>
-      <c r="N24" s="20">
+      <c r="N24" s="21">
         <v>60</v>
       </c>
     </row>
     <row r="25" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I25" s="19"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
     </row>
     <row r="26" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I26" s="19" t="s">
+      <c r="I26" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="J26" s="20">
+      <c r="J26" s="21">
         <v>19</v>
       </c>
-      <c r="K26" s="20">
+      <c r="K26" s="21">
         <v>76</v>
       </c>
-      <c r="L26" s="20">
+      <c r="L26" s="21">
         <v>4</v>
       </c>
-      <c r="M26" s="20">
+      <c r="M26" s="21">
         <v>76</v>
       </c>
-      <c r="N26" s="20">
+      <c r="N26" s="21">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I27" s="19"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
     </row>
     <row r="28" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I28" s="19" t="s">
+      <c r="I28" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J28" s="20">
+      <c r="J28" s="21">
         <v>96</v>
       </c>
-      <c r="K28" s="20">
+      <c r="K28" s="21">
         <v>370</v>
       </c>
-      <c r="L28" s="20">
+      <c r="L28" s="21">
         <v>4</v>
       </c>
-      <c r="M28" s="20">
+      <c r="M28" s="21">
         <v>310</v>
       </c>
-      <c r="N28" s="20">
+      <c r="N28" s="21">
         <v>60</v>
       </c>
     </row>
     <row r="29" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I29" s="19"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
     </row>
     <row r="30" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I30" s="19" t="s">
+      <c r="I30" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J30" s="20">
+      <c r="J30" s="21">
         <v>28</v>
       </c>
-      <c r="K30" s="20">
+      <c r="K30" s="21">
         <v>110</v>
       </c>
-      <c r="L30" s="20">
+      <c r="L30" s="21">
         <v>4</v>
       </c>
-      <c r="M30" s="20">
+      <c r="M30" s="21">
         <v>62</v>
       </c>
-      <c r="N30" s="20">
+      <c r="N30" s="21">
         <v>48</v>
       </c>
     </row>
     <row r="31" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I31" s="19"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
     </row>
     <row r="32" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I32" s="19" t="s">
+      <c r="I32" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="J32" s="20">
+      <c r="J32" s="21">
         <v>25</v>
       </c>
-      <c r="K32" s="20">
+      <c r="K32" s="21">
         <v>94</v>
       </c>
-      <c r="L32" s="20">
+      <c r="L32" s="21">
         <v>4</v>
       </c>
-      <c r="M32" s="20">
+      <c r="M32" s="21">
         <v>94</v>
       </c>
-      <c r="N32" s="20">
+      <c r="N32" s="21">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I33" s="19"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="20"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="21"/>
     </row>
     <row r="34" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I34" s="19" t="s">
+      <c r="I34" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J34" s="21">
+      <c r="J34" s="19">
         <v>306</v>
       </c>
-      <c r="K34" s="21">
+      <c r="K34" s="19">
         <v>1166</v>
       </c>
-      <c r="L34" s="22"/>
-      <c r="M34" s="20">
+      <c r="L34" s="20"/>
+      <c r="M34" s="21">
         <v>778</v>
       </c>
-      <c r="N34" s="20">
+      <c r="N34" s="21">
         <v>388</v>
       </c>
     </row>
     <row r="35" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="I35" s="19"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="20"/>
-      <c r="N35" s="20"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="K34:K35"/>
-    <mergeCell ref="L34:L35"/>
-    <mergeCell ref="M34:M35"/>
-    <mergeCell ref="N34:N35"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="L32:L33"/>
-    <mergeCell ref="M32:M33"/>
-    <mergeCell ref="N32:N33"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="N30:N31"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="N28:N29"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="J18:J21"/>
+    <mergeCell ref="K18:K21"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="K22:K23"/>
     <mergeCell ref="N26:N27"/>
     <mergeCell ref="L22:L23"/>
     <mergeCell ref="M22:M23"/>
@@ -2887,12 +2916,35 @@
     <mergeCell ref="L24:L25"/>
     <mergeCell ref="M24:M25"/>
     <mergeCell ref="N24:N25"/>
-    <mergeCell ref="I18:I21"/>
-    <mergeCell ref="J18:J21"/>
-    <mergeCell ref="K18:K21"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="N30:N31"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="N28:N29"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="N34:N35"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="M32:M33"/>
+    <mergeCell ref="N32:N33"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="L34:L35"/>
+    <mergeCell ref="M34:M35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>